<commit_message>
update indexing times plot with qdrant and last value of pinecone
</commit_message>
<xml_diff>
--- a/Data/Analysis/Indexing Results.xlsx
+++ b/Data/Analysis/Indexing Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="give the excel resulting data i" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="data" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="32">
   <si>
     <t>VectorStore</t>
   </si>
@@ -28,6 +28,16 @@
     <t>corpus_1</t>
   </si>
   <si>
+    <t>Qdrant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1875.1019s
+</t>
+  </si>
+  <si>
+    <t>Batch_size=500</t>
+  </si>
+  <si>
     <t>Faiss</t>
   </si>
   <si>
@@ -40,6 +50,10 @@
     <t>OpenSearch</t>
   </si>
   <si>
+    <t xml:space="preserve">corpus_1:Total Indexed Documents (Chunks): 141964
+</t>
+  </si>
+  <si>
     <t>Pinecone</t>
   </si>
   <si>
@@ -55,25 +69,50 @@
     <t>Original Larger Corpus</t>
   </si>
   <si>
+    <t xml:space="preserve">corpus_2:Total Indexed Documents (Chunks): 284115
+</t>
+  </si>
+  <si>
     <t>corpus_3</t>
   </si>
   <si>
+    <t>5098.6360s</t>
+  </si>
+  <si>
     <t>Original Smaller Corpus</t>
   </si>
   <si>
+    <t xml:space="preserve">corpus_3:Indexed Documents (Chunks): 426563
+</t>
+  </si>
+  <si>
     <t>corpus_4</t>
   </si>
   <si>
+    <t xml:space="preserve">corpus_4:otal Indexed Documents (Chunks): 568811
+</t>
+  </si>
+  <si>
     <t>corpus_5</t>
   </si>
   <si>
+    <t>corpus_5: Total Indexed Documents (Chunks): 710741</t>
+  </si>
+  <si>
     <t>corpus_6</t>
   </si>
   <si>
-    <t>Missing Pinecone, Qdrant</t>
+    <t xml:space="preserve">corpus_6:Total Indexed Documents (Chunks): 853086
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10765.1080s</t>
   </si>
   <si>
     <t>corpus_7</t>
+  </si>
+  <si>
+    <t>corpus_7:  Indexed Documents (Chunks): 995399</t>
   </si>
 </sst>
 </file>
@@ -329,6 +368,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="22.63"/>
+    <col customWidth="1" min="4" max="4" width="27.5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1"/>
@@ -352,14 +395,12 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
-        <v>1592.2479</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1706.8407</v>
-      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -367,33 +408,34 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>1648.2282</v>
+        <v>1592.2479</v>
       </c>
       <c r="D3" s="1">
         <v>1706.8407</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>1724.7053</v>
+        <v>1648.2282</v>
       </c>
       <c r="D4" s="1">
         <v>1706.8407</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -401,16 +443,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
-        <v>1733.1885</v>
+        <v>1724.7053</v>
       </c>
       <c r="D5" s="1">
         <v>1706.8407</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -418,166 +463,165 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
-        <v>1732.4131</v>
+        <v>1733.1885</v>
       </c>
       <c r="D6" s="1">
         <v>1706.8407</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1732.4131</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1706.8407</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3112.5788</v>
-      </c>
-      <c r="D8" s="1">
-        <v>3413.7405</v>
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
-        <v>3293.0413</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3413.7405</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>4144.72</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>3483.7279</v>
+        <v>3112.5788</v>
       </c>
       <c r="D10" s="1">
         <v>3413.7405</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1">
-        <v>3484.5604</v>
+        <v>3293.0413</v>
       </c>
       <c r="D11" s="1">
         <v>3413.7405</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1">
-        <v>3690.795</v>
+        <v>3483.7279</v>
       </c>
       <c r="D12" s="1">
         <v>3413.7405</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3484.5604</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3413.7405</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1">
-        <v>4614.0377</v>
+        <v>3690.795</v>
       </c>
       <c r="D14" s="1">
-        <v>5101.6401</v>
+        <v>3413.7405</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1">
-        <v>5052.4943</v>
-      </c>
-      <c r="D15" s="1">
-        <v>5101.6401</v>
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>15</v>
@@ -585,137 +629,143 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="1">
-        <v>5200.1994</v>
-      </c>
-      <c r="D16" s="1">
-        <v>5101.6401</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="1">
-        <v>5301.9771</v>
+        <v>4614.0377</v>
       </c>
       <c r="D17" s="1">
         <v>5101.6401</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>5339.5912</v>
+        <v>5052.4943</v>
       </c>
       <c r="D18" s="1">
         <v>5101.6401</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5200.1994</v>
+      </c>
+      <c r="D19" s="1">
+        <v>5101.6401</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C20" s="1">
-        <v>6378.1634</v>
+        <v>5301.9771</v>
       </c>
       <c r="D20" s="1">
-        <v>6884.8402</v>
+        <v>5101.6401</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>6750.3368</v>
+        <v>5339.5912</v>
       </c>
       <c r="D21" s="1">
-        <v>6884.8402</v>
+        <v>5101.6401</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="1">
-        <v>7085.6162</v>
-      </c>
-      <c r="D22" s="1">
-        <v>6884.8402</v>
+        <v>15</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1">
-        <v>7086.7322</v>
-      </c>
-      <c r="D23" s="1">
-        <v>6884.8402</v>
-      </c>
+        <v>6836.3935</v>
+      </c>
+      <c r="D23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1">
-        <v>7123.3507</v>
+        <v>6378.1634</v>
       </c>
       <c r="D24" s="1">
         <v>6884.8402</v>
@@ -723,259 +773,365 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C25" s="1">
+        <v>6750.3368</v>
+      </c>
+      <c r="D25" s="1">
+        <v>6884.8402</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1">
-        <v>7032.6974</v>
+        <v>7085.6162</v>
       </c>
       <c r="D26" s="1">
-        <v>8365.6231</v>
+        <v>6884.8402</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1">
-        <v>7507.2509</v>
+        <v>7086.7322</v>
       </c>
       <c r="D27" s="1">
-        <v>8365.6231</v>
+        <v>6884.8402</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1">
-        <v>8374.4418</v>
+        <v>7123.3507</v>
       </c>
       <c r="D28" s="1">
-        <v>8365.6231</v>
+        <v>6884.8402</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1">
-        <v>8893.7857</v>
-      </c>
-      <c r="D29" s="1">
-        <v>8365.6231</v>
+        <v>15</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C30" s="1">
-        <v>8969.9517</v>
-      </c>
-      <c r="D30" s="1">
-        <v>8365.6231</v>
-      </c>
+        <v>10626.6383</v>
+      </c>
+      <c r="D30" s="1"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="C31" s="1">
+        <v>7032.6974</v>
+      </c>
+      <c r="D31" s="1">
+        <v>8365.6231</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C32" s="1">
-        <v>9313.5707</v>
+        <v>7507.2509</v>
       </c>
       <c r="D32" s="1">
-        <v>10378.9021</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>19</v>
+        <v>8365.6231</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1">
-        <v>10061.7689</v>
+        <v>8374.4418</v>
       </c>
       <c r="D33" s="1">
-        <v>10378.9021</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>19</v>
+        <v>8365.6231</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C34" s="1">
-        <v>10587.7599</v>
+        <v>8893.7857</v>
       </c>
       <c r="D34" s="1">
-        <v>10378.9021</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>19</v>
+        <v>8365.6231</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C35" s="1">
-        <v>11552.5189</v>
+        <v>8969.9517</v>
       </c>
       <c r="D35" s="1">
-        <v>10378.9021</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>19</v>
+        <v>8365.6231</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="1">
-        <v>10939.6636</v>
-      </c>
-      <c r="D37" s="1">
-        <v>12567.3378</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>10222.3496</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C38" s="1">
-        <v>12585.5039</v>
+        <v>9313.5707</v>
       </c>
       <c r="D38" s="1">
-        <v>12567.3378</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>19</v>
+        <v>10378.9021</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C39" s="1">
-        <v>12585.5039</v>
+        <v>10061.7689</v>
       </c>
       <c r="D39" s="1">
-        <v>12567.3378</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>19</v>
+        <v>10378.9021</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="1">
+        <v>10587.7599</v>
+      </c>
+      <c r="D40" s="1">
+        <v>10378.9021</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="1">
+        <v>11552.5189</v>
+      </c>
+      <c r="D41" s="1">
+        <v>10378.9021</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1">
+        <v>11811.6426</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="1">
+        <v>10939.6636</v>
+      </c>
+      <c r="D45" s="1">
+        <v>12567.3378</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C46" s="1">
+        <v>12585.5039</v>
+      </c>
+      <c r="D46" s="1">
+        <v>12567.3378</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="1">
+        <v>12585.5039</v>
+      </c>
+      <c r="D47" s="1">
+        <v>12567.3378</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="1">
         <v>14158.6774</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D48" s="1">
         <v>12567.3378</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>19</v>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="1">
+        <v>12549.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>